<commit_message>
Added Modules (Financeiro, Clientes)
</commit_message>
<xml_diff>
--- a/taskList.xlsx
+++ b/taskList.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vini2\Desktop\JJP Data Intelligence\Projetos\Projetos Ativos\3e Consulting\BI4U\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A130AA79-5402-4B3D-B773-332F3F1B3C5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454F82DE-0E04-4BE6-8E04-7DA9581C3C9A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6C27AEC3-B6D4-43E8-A980-4A3197A4638C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet name="Funcionários" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,8 +30,36 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Vinícius Lavrador</author>
+  </authors>
+  <commentList>
+    <comment ref="F25" authorId="0" shapeId="0" xr:uid="{4E0D64DE-6979-4567-9484-32F25179C898}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Vinícius Lavrador:
+Dentro do Menu do módulo Financeiro, teremos 3 opcoes: Lançamentos, Visualizar Lançamentos e  Fluxo de Caixa. 
+Dentro de Fluxo de Caixa teremos um submenu para escolher o periodo entre Semana, Mês, Trimestre, Semestre e Ano.
+Dentro de Lançamentos teremos um modal com o formulário de lançamento para receita ou despesa e um checkbox para escolher entre receita e despesa. Caso seja receita, habilita um campo para escolha de cliente.
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Tela inicial do sistema, deve ser aquela azul que lhe passei com o logo da GAP no meio.</t>
   </si>
@@ -81,9 +109,6 @@
     <t>No resumo de cadastro que é apresentados após pesquisa por CPF trocar o campo "funcionário ativo" por Status. Para o Status apresentar as seguintes opções: Admitido ou Contratado, Afastado, Demitido e Férias.</t>
   </si>
   <si>
-    <t>Tasks</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -91,13 +116,49 @@
   </si>
   <si>
     <t>Progress</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Criar visualização geral de funcionários, contendo apenas informações básicas</t>
+  </si>
+  <si>
+    <t>Desligamento de Funcionários</t>
+  </si>
+  <si>
+    <t>Terminar Back-End Financeiro</t>
+  </si>
+  <si>
+    <t>Estruturar Front-End Financeiro</t>
+  </si>
+  <si>
+    <t>Botão de Escolha SEG ou EIRELI - Empresa Contratante - CB - Funcionário</t>
+  </si>
+  <si>
+    <t>Estruturar Front-End Clientes</t>
+  </si>
+  <si>
+    <t>Estruturar Back-End Clientes - Esperar informações de Campo do Thiago</t>
+  </si>
+  <si>
+    <t>Adicionar Mensagem de Erros nas Informações Bancárias</t>
+  </si>
+  <si>
+    <t>Simulação do Módulo Financeiro funcionando</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,8 +181,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -131,6 +207,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -202,7 +296,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -219,14 +313,68 @@
     <xf numFmtId="10" fontId="2" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -542,268 +690,542 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44BB84BF-369C-45E9-A482-8E63367EB510}">
-  <dimension ref="A2:L20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44BB84BF-369C-45E9-A482-8E63367EB510}">
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="67.109375" style="1" customWidth="1"/>
-    <col min="7" max="11" width="8.88671875" style="1"/>
-    <col min="12" max="12" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="7" max="7" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="13" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F1" s="10"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="E2" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="F2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="I2" s="21"/>
+    </row>
+    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1"/>
+      <c r="E3" s="14">
+        <v>1</v>
+      </c>
+      <c r="F3" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="16">
+        <v>43560</v>
+      </c>
+      <c r="H3" s="17">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <f>H3</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" s="5">
+        <f>SUM(H3:H28)/COUNTA(H3:H28)</f>
+        <v>0.73076923076923073</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A4" s="1"/>
+      <c r="E4" s="14">
+        <v>2</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="16">
+        <v>43560</v>
+      </c>
+      <c r="H4" s="15">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <f t="shared" ref="I4:I28" si="0">H4</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1"/>
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="1"/>
+      <c r="E6" s="11">
+        <v>4</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="13">
+        <v>43560</v>
+      </c>
+      <c r="H6" s="12">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="M6" s="10"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="1"/>
+      <c r="E7" s="7">
+        <v>5</v>
+      </c>
+      <c r="F7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="1"/>
+      <c r="E8" s="7">
+        <v>6</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="G8" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="1"/>
+      <c r="E9" s="7">
+        <v>7</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G9" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
+      <c r="I9" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="1"/>
+      <c r="E10" s="7">
+        <v>8</v>
+      </c>
+      <c r="F10" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H10" s="8">
+        <v>1</v>
+      </c>
+      <c r="I10" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="1"/>
+      <c r="E11" s="7">
+        <v>9</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G11" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H11" s="8">
+        <v>1</v>
+      </c>
+      <c r="I11" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="1"/>
+      <c r="E12" s="7">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="G12" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H12" s="8">
+        <v>1</v>
+      </c>
+      <c r="I12" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="1"/>
+      <c r="E13" s="7">
+        <v>11</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="1"/>
+      <c r="E14" s="7">
+        <v>12</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G14" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H14" s="8">
+        <v>1</v>
+      </c>
+      <c r="I14" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="1"/>
+      <c r="E15" s="7">
+        <v>13</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H15" s="8">
+        <v>1</v>
+      </c>
+      <c r="I15" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A16" s="1"/>
+      <c r="E16" s="7">
+        <v>14</v>
+      </c>
+      <c r="F16" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="8"/>
-    </row>
-    <row r="3" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="F3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="6">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
-        <f>G3</f>
-        <v>0</v>
-      </c>
-      <c r="K3" s="4" t="s">
+      <c r="G16" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H16" s="8">
+        <v>1</v>
+      </c>
+      <c r="I16" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="1"/>
+      <c r="E17" s="7">
+        <v>15</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H17" s="8">
+        <v>1</v>
+      </c>
+      <c r="I17" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="E18" s="7">
+        <v>16</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H18" s="8">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="E19" s="7">
+        <v>17</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H19" s="8">
+        <v>1</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="E20" s="7">
+        <v>18</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="G20" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H20" s="8">
+        <v>1</v>
+      </c>
+      <c r="I20" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="E21" s="7">
         <v>19</v>
       </c>
-      <c r="L3" s="5">
-        <f>SUM(G3:G19)/COUNTA(G3:G19)</f>
-        <v>0.23529411764705882</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1"/>
-      <c r="F4" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
-        <f t="shared" ref="H4:H19" si="0">G4</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="F5" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G5" s="3">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="F6" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="1"/>
-      <c r="F7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="G7" s="3">
-        <v>1</v>
-      </c>
-      <c r="H7" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="1"/>
-      <c r="F8" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-      <c r="F9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-      <c r="F10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-      <c r="F11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-      <c r="F12" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1</v>
-      </c>
-      <c r="H12" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="F13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-      <c r="F14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-      <c r="F15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-      <c r="F16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1</v>
-      </c>
-      <c r="H16" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-      <c r="F17" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-      <c r="F18" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="F19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0</v>
-      </c>
-      <c r="H19" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
+      <c r="F21" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H21" s="8">
+        <v>1</v>
+      </c>
+      <c r="I21" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E22" s="24">
+        <v>20</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G22" s="25">
+        <v>43567</v>
+      </c>
+      <c r="H22" s="26">
+        <v>1</v>
+      </c>
+      <c r="I22" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E23" s="18">
+        <v>21</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G23" s="19">
+        <v>43567</v>
+      </c>
+      <c r="H23" s="23">
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E24" s="18">
+        <v>22</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="G24" s="19">
+        <v>43567</v>
+      </c>
+      <c r="H24" s="23">
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E25" s="18">
+        <v>23</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="G25" s="19">
+        <v>43567</v>
+      </c>
+      <c r="H25" s="23">
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E26" s="18">
+        <v>24</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>27</v>
+      </c>
+      <c r="G26" s="19">
+        <v>43567</v>
+      </c>
+      <c r="H26" s="23">
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E27" s="24">
+        <v>25</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="25">
+        <v>43567</v>
+      </c>
+      <c r="H27" s="26">
+        <v>1</v>
+      </c>
+      <c r="I27" s="3">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="E28" s="18">
+        <v>26</v>
+      </c>
+      <c r="F28" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="G28" s="19">
+        <v>43567</v>
+      </c>
+      <c r="H28" s="23">
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="H2:I2"/>
   </mergeCells>
-  <conditionalFormatting sqref="H3:H19">
-    <cfRule type="iconSet" priority="1">
+  <conditionalFormatting sqref="I3:I28">
+    <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="33"/>
@@ -813,5 +1235,6 @@
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adjusts in Income, Expense Forms
</commit_message>
<xml_diff>
--- a/taskList.xlsx
+++ b/taskList.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vini2\Desktop\JJP Data Intelligence\Projetos\Projetos Ativos\3e Consulting\BI4U\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{454F82DE-0E04-4BE6-8E04-7DA9581C3C9A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23796F1E-242F-4B5E-8517-0DEC5D2D9F5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6C27AEC3-B6D4-43E8-A980-4A3197A4638C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Funcionários" sheetId="1" r:id="rId1"/>
+    <sheet name="ToDo" sheetId="1" r:id="rId1"/>
+    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,12 +55,82 @@
         </r>
       </text>
     </comment>
+    <comment ref="F29" authorId="0" shapeId="0" xr:uid="{6A46FE84-97EC-485C-BF72-95A61F8CE1B1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Vinícius Lavrador:
+Cartao Débito
+Cartão Crédito
+Boleto
+Transferência
+Dinheiro
+Depósito</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F32" authorId="0" shapeId="0" xr:uid="{CCDC2C71-F252-40C5-815B-2D61C235DBAA}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Vinícius Lavrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Admin do Cliente - Permissão Total Dentre os Aplicativos de Usuário.
+Usuário Comum - Acesso de Visualização do Funcionário.
+Usuário Intermediário - Acesso de Visualização e Escrita em todos os Aplicativos de Usuário</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F33" authorId="0" shapeId="0" xr:uid="{D73D198A-C6B0-4B27-AEC1-C5397875CFB8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Vinícius Lavrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No formulario de Receita e Despesa, teremos 2 paginas. A primeira com informações de Detalhes Financeiros (ID. Venda, Classificação De Receita, Produto ou Serviço, Quantidade, Valor Unitário do Produto ou Serviço) com o máximo de linhas possíveis sem que o scroll seja necessário. A segunda com o restante das informações que consernem o lançamento.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Tela inicial do sistema, deve ser aquela azul que lhe passei com o logo da GAP no meio.</t>
   </si>
@@ -152,13 +223,70 @@
   </si>
   <si>
     <t>Simulação do Módulo Financeiro funcionando</t>
+  </si>
+  <si>
+    <t>Aguardando informações sobre metadados do backend virem do Thiago.</t>
+  </si>
+  <si>
+    <t>Boleto</t>
+  </si>
+  <si>
+    <t>Transferencia</t>
+  </si>
+  <si>
+    <t>Cartão de Débito</t>
+  </si>
+  <si>
+    <t>Cartão de Crédito</t>
+  </si>
+  <si>
+    <t>Dinheiro</t>
+  </si>
+  <si>
+    <t>Alteração de Tipos de Forma de Pagamento</t>
+  </si>
+  <si>
+    <t>Criação de Página para uso Anônimo PARA Clientes da Empresa</t>
+  </si>
+  <si>
+    <t>Criação de Página de Prospect para Clientes da empresa</t>
+  </si>
+  <si>
+    <t>Criação de 2 Grupos de Autorização e flag Staff no Django</t>
+  </si>
+  <si>
+    <t>No formulario de Receita e Despesa, teremos 2 paginas. A primeira com informações de Destalhes Financeiros (ID. Venda, Classificação De Receita, Produto ou Serviço, Quantidade, Valor Unitário do Produto ou Serviço)</t>
+  </si>
+  <si>
+    <t>Ajustar Formulários de Lançamentos Receita e Despesa</t>
+  </si>
+  <si>
+    <t>Ajustar Formulários de Lançamentos Receita e Despesa para o Valor total refletir a soma dos produtos e serviços menos o percentual de desconto</t>
+  </si>
+  <si>
+    <t>Ao Abrir o Menu, Fechar os Submenus de Lançamentos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No Fluxo de Caixa, mostrar visões dos seguintes períodos: -Diário(Escolhe Mês e Ano), Semana(Sumarização por Semana, Escolhe mês e ano), Ultimos 3 Meses(Sumarização por Mês, sem escolhas), Ultimos 6 Meses (idem ao anterior), Ultimos 12 Meses(Sumarização por Mês) </t>
+  </si>
+  <si>
+    <t>Arrumar as Casas Decimais</t>
+  </si>
+  <si>
+    <t>Revisão Geral Ortográfica</t>
+  </si>
+  <si>
+    <t>Adicionar Dependentes no Módulo Funcionário</t>
+  </si>
+  <si>
+    <t>Pesquisar e Criar Método de exportação das diferentes vizualizações do módulo financeiro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,8 +324,21 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -218,18 +359,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -278,25 +413,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -328,52 +450,73 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="12" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -691,10 +834,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44BB84BF-369C-45E9-A482-8E63367EB510}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -702,7 +845,9 @@
     <col min="2" max="5" width="8.88671875" style="1"/>
     <col min="6" max="6" width="67.109375" style="1" customWidth="1"/>
     <col min="7" max="7" width="10.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="8.88671875" style="1"/>
+    <col min="8" max="9" width="8.88671875" style="1"/>
+    <col min="10" max="10" width="25.33203125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" style="1"/>
     <col min="12" max="13" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -720,55 +865,58 @@
       <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="21"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
     </row>
     <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
-      <c r="E3" s="14">
-        <v>1</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="16">
-        <v>43560</v>
-      </c>
-      <c r="H3" s="17">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3">
+      <c r="E3" s="7">
+        <v>1</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H3" s="18">
+        <v>1</v>
+      </c>
+      <c r="I3" s="12">
         <f>H3</f>
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="J3" s="13"/>
       <c r="L3" s="4" t="s">
         <v>18</v>
       </c>
       <c r="M3" s="5">
         <f>SUM(H3:H28)/COUNTA(H3:H28)</f>
-        <v>0.73076923076923073</v>
+        <v>0.92307692307692313</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="1"/>
-      <c r="E4" s="14">
+      <c r="E4" s="7">
         <v>2</v>
       </c>
-      <c r="F4" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="G4" s="16">
-        <v>43560</v>
-      </c>
-      <c r="H4" s="15">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3">
-        <f t="shared" ref="I4:I28" si="0">H4</f>
-        <v>0</v>
-      </c>
+      <c r="F4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G4" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H4" s="19">
+        <v>1</v>
+      </c>
+      <c r="I4" s="12">
+        <f t="shared" ref="I4:I40" si="0">H4</f>
+        <v>1</v>
+      </c>
+      <c r="J4" s="13"/>
     </row>
     <row r="5" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
@@ -781,32 +929,34 @@
       <c r="G5" s="9">
         <v>43560</v>
       </c>
-      <c r="H5" s="8">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="H5" s="19">
+        <v>1</v>
+      </c>
+      <c r="I5" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J5" s="13"/>
     </row>
     <row r="6" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="E6" s="11">
+      <c r="E6" s="7">
         <v>4</v>
       </c>
-      <c r="F6" s="12" t="s">
+      <c r="F6" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="13">
-        <v>43560</v>
-      </c>
-      <c r="H6" s="12">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="G6" s="9">
+        <v>43560</v>
+      </c>
+      <c r="H6" s="19">
+        <v>1</v>
+      </c>
+      <c r="I6" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J6" s="13"/>
       <c r="M6" s="10"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
@@ -820,13 +970,14 @@
       <c r="G7" s="9">
         <v>43560</v>
       </c>
-      <c r="H7" s="8">
-        <v>1</v>
-      </c>
-      <c r="I7" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="H7" s="19">
+        <v>1</v>
+      </c>
+      <c r="I7" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
@@ -839,13 +990,14 @@
       <c r="G8" s="9">
         <v>43560</v>
       </c>
-      <c r="H8" s="8">
-        <v>1</v>
-      </c>
-      <c r="I8" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="H8" s="19">
+        <v>1</v>
+      </c>
+      <c r="I8" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J8" s="13"/>
     </row>
     <row r="9" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
@@ -858,13 +1010,14 @@
       <c r="G9" s="9">
         <v>43560</v>
       </c>
-      <c r="H9" s="8">
-        <v>1</v>
-      </c>
-      <c r="I9" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="H9" s="19">
+        <v>1</v>
+      </c>
+      <c r="I9" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J9" s="13"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
@@ -877,13 +1030,14 @@
       <c r="G10" s="9">
         <v>43560</v>
       </c>
-      <c r="H10" s="8">
-        <v>1</v>
-      </c>
-      <c r="I10" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="H10" s="19">
+        <v>1</v>
+      </c>
+      <c r="I10" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J10" s="13"/>
     </row>
     <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
@@ -896,13 +1050,14 @@
       <c r="G11" s="9">
         <v>43560</v>
       </c>
-      <c r="H11" s="8">
-        <v>1</v>
-      </c>
-      <c r="I11" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="H11" s="19">
+        <v>1</v>
+      </c>
+      <c r="I11" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J11" s="13"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
@@ -915,13 +1070,14 @@
       <c r="G12" s="9">
         <v>43560</v>
       </c>
-      <c r="H12" s="8">
-        <v>1</v>
-      </c>
-      <c r="I12" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="H12" s="19">
+        <v>1</v>
+      </c>
+      <c r="I12" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J12" s="13"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
@@ -934,13 +1090,14 @@
       <c r="G13" s="9">
         <v>43560</v>
       </c>
-      <c r="H13" s="8">
-        <v>1</v>
-      </c>
-      <c r="I13" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="H13" s="19">
+        <v>1</v>
+      </c>
+      <c r="I13" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J13" s="13"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
@@ -953,13 +1110,14 @@
       <c r="G14" s="9">
         <v>43560</v>
       </c>
-      <c r="H14" s="8">
-        <v>1</v>
-      </c>
-      <c r="I14" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="H14" s="19">
+        <v>1</v>
+      </c>
+      <c r="I14" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J14" s="13"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
@@ -972,13 +1130,14 @@
       <c r="G15" s="9">
         <v>43560</v>
       </c>
-      <c r="H15" s="8">
-        <v>1</v>
-      </c>
-      <c r="I15" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
+      <c r="H15" s="19">
+        <v>1</v>
+      </c>
+      <c r="I15" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J15" s="13"/>
     </row>
     <row r="16" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
@@ -991,15 +1150,16 @@
       <c r="G16" s="9">
         <v>43560</v>
       </c>
-      <c r="H16" s="8">
-        <v>1</v>
-      </c>
-      <c r="I16" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H16" s="19">
+        <v>1</v>
+      </c>
+      <c r="I16" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J16" s="13"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="E17" s="7">
         <v>15</v>
@@ -1010,15 +1170,16 @@
       <c r="G17" s="9">
         <v>43560</v>
       </c>
-      <c r="H17" s="8">
-        <v>1</v>
-      </c>
-      <c r="I17" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H17" s="19">
+        <v>1</v>
+      </c>
+      <c r="I17" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J17" s="13"/>
+    </row>
+    <row r="18" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="E18" s="7">
         <v>16</v>
@@ -1029,15 +1190,16 @@
       <c r="G18" s="9">
         <v>43560</v>
       </c>
-      <c r="H18" s="8">
-        <v>1</v>
-      </c>
-      <c r="I18" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="H18" s="19">
+        <v>1</v>
+      </c>
+      <c r="I18" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="E19" s="7">
         <v>17</v>
@@ -1048,15 +1210,16 @@
       <c r="G19" s="9">
         <v>43560</v>
       </c>
-      <c r="H19" s="8">
-        <v>1</v>
-      </c>
-      <c r="I19" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H19" s="19">
+        <v>1</v>
+      </c>
+      <c r="I19" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J19" s="13"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="E20" s="7">
         <v>18</v>
@@ -1067,15 +1230,16 @@
       <c r="G20" s="9">
         <v>43560</v>
       </c>
-      <c r="H20" s="8">
-        <v>1</v>
-      </c>
-      <c r="I20" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="H20" s="19">
+        <v>1</v>
+      </c>
+      <c r="I20" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J20" s="13"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="E21" s="7">
         <v>19</v>
@@ -1086,150 +1250,389 @@
       <c r="G21" s="9">
         <v>43560</v>
       </c>
-      <c r="H21" s="8">
-        <v>1</v>
-      </c>
-      <c r="I21" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E22" s="24">
+      <c r="H21" s="19">
+        <v>1</v>
+      </c>
+      <c r="I21" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J21" s="13"/>
+      <c r="L21" s="10"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E22" s="14">
         <v>20</v>
       </c>
       <c r="F22" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G22" s="25">
+      <c r="G22" s="15">
         <v>43567</v>
       </c>
-      <c r="H22" s="26">
-        <v>1</v>
-      </c>
-      <c r="I22" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E23" s="18">
+      <c r="H22" s="19">
+        <v>1</v>
+      </c>
+      <c r="I22" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J22" s="13"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E23" s="14">
         <v>21</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G23" s="19">
+      <c r="G23" s="15">
         <v>43567</v>
       </c>
-      <c r="H23" s="23">
-        <v>0</v>
-      </c>
-      <c r="I23" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E24" s="18">
+      <c r="H23" s="19">
+        <v>1</v>
+      </c>
+      <c r="I23" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J23" s="13"/>
+    </row>
+    <row r="24" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E24" s="13">
         <v>22</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G24" s="19">
+      <c r="G24" s="16">
         <v>43567</v>
       </c>
-      <c r="H24" s="23">
-        <v>0</v>
-      </c>
-      <c r="I24" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E25" s="18">
+      <c r="H24" s="17">
+        <v>0</v>
+      </c>
+      <c r="I24" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J24" s="13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E25" s="14">
         <v>23</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="19">
+      <c r="G25" s="15">
         <v>43567</v>
       </c>
-      <c r="H25" s="23">
-        <v>0</v>
-      </c>
-      <c r="I25" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E26" s="18">
+      <c r="H25" s="19">
+        <v>1</v>
+      </c>
+      <c r="I25" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J25" s="13"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E26" s="13">
         <v>24</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F26" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="19">
+      <c r="G26" s="16">
         <v>43567</v>
       </c>
-      <c r="H26" s="23">
-        <v>0</v>
-      </c>
-      <c r="I26" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E27" s="24">
+      <c r="H26" s="17">
+        <v>0</v>
+      </c>
+      <c r="I26" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="13"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E27" s="14">
         <v>25</v>
       </c>
       <c r="F27" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G27" s="25">
+      <c r="G27" s="15">
         <v>43567</v>
       </c>
-      <c r="H27" s="26">
-        <v>1</v>
-      </c>
-      <c r="I27" s="3">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="E28" s="18">
+      <c r="H27" s="19">
+        <v>1</v>
+      </c>
+      <c r="I27" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J27" s="13"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E28" s="14">
         <v>26</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="G28" s="19">
+      <c r="G28" s="15">
         <v>43567</v>
       </c>
-      <c r="H28" s="23">
-        <v>0</v>
-      </c>
-      <c r="I28" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
+      <c r="H28" s="19">
+        <v>1</v>
+      </c>
+      <c r="I28" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J28" s="13"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E29" s="26">
+        <v>27</v>
+      </c>
+      <c r="F29" s="25" t="s">
+        <v>37</v>
+      </c>
+      <c r="G29" s="24">
+        <v>43574</v>
+      </c>
+      <c r="H29" s="8">
+        <v>1</v>
+      </c>
+      <c r="I29" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J29" s="20"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E30" s="29">
+        <v>28</v>
+      </c>
+      <c r="F30" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="G30" s="31">
+        <v>43574</v>
+      </c>
+      <c r="H30" s="32">
+        <v>-1</v>
+      </c>
+      <c r="I30" s="12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="J30" s="20"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E31" s="29">
+        <v>29</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="31">
+        <v>43574</v>
+      </c>
+      <c r="H31" s="32">
+        <v>-1</v>
+      </c>
+      <c r="I31" s="12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="J31" s="20"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E32" s="29">
+        <v>30</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="G32" s="31">
+        <v>43574</v>
+      </c>
+      <c r="H32" s="32">
+        <v>-1</v>
+      </c>
+      <c r="I32" s="12">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="J32" s="20"/>
+    </row>
+    <row r="33" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E33" s="27">
+        <v>31</v>
+      </c>
+      <c r="F33" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33" s="21">
+        <v>43574</v>
+      </c>
+      <c r="H33" s="3">
+        <v>0</v>
+      </c>
+      <c r="I33" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J33" s="20"/>
+    </row>
+    <row r="34" spans="5:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E34" s="28">
+        <v>32</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="G34" s="16">
+        <v>43574</v>
+      </c>
+      <c r="H34" s="3">
+        <v>0</v>
+      </c>
+      <c r="I34" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J34" s="20"/>
+    </row>
+    <row r="35" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E35" s="27">
+        <v>33</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G35" s="21">
+        <v>43574</v>
+      </c>
+      <c r="H35" s="3">
+        <v>0</v>
+      </c>
+      <c r="I35" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="20"/>
+    </row>
+    <row r="36" spans="5:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E36" s="28">
+        <v>34</v>
+      </c>
+      <c r="F36" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="G36" s="16">
+        <v>43574</v>
+      </c>
+      <c r="H36" s="3">
+        <v>0</v>
+      </c>
+      <c r="I36" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J36" s="20"/>
+    </row>
+    <row r="37" spans="5:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E37" s="28">
+        <v>35</v>
+      </c>
+      <c r="F37" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="G37" s="16">
+        <v>43574</v>
+      </c>
+      <c r="H37" s="3">
+        <v>0</v>
+      </c>
+      <c r="I37" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E38" s="27">
+        <v>36</v>
+      </c>
+      <c r="F38" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="21">
+        <v>43574</v>
+      </c>
+      <c r="H38" s="3">
+        <v>0</v>
+      </c>
+      <c r="I38" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E39" s="27">
+        <v>37</v>
+      </c>
+      <c r="F39" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="G39" s="21">
+        <v>43574</v>
+      </c>
+      <c r="H39" s="3">
+        <v>0</v>
+      </c>
+      <c r="I39" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J39" s="20"/>
+    </row>
+    <row r="40" spans="5:10" x14ac:dyDescent="0.3">
+      <c r="E40" s="27">
+        <v>38</v>
+      </c>
+      <c r="F40" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="G40" s="21">
+        <v>43574</v>
+      </c>
+      <c r="H40" s="23">
+        <v>0</v>
+      </c>
+      <c r="I40" s="3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="H2:J2"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:I28">
+  <conditionalFormatting sqref="I3:I40">
     <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
-        <cfvo type="percent" val="33"/>
-        <cfvo type="percent" val="67"/>
+        <cfvo type="percent" val="0" gte="0"/>
+        <cfvo type="num" val="1"/>
       </iconSet>
     </cfRule>
   </conditionalFormatting>
@@ -1237,4 +1640,50 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134A7412-1C13-47AD-96AC-2FA85A2170B3}">
+  <dimension ref="A1:F5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="40.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Stable Version Uploaded to Python Anywhere on 12/05/2019 - Version 1.0.0
</commit_message>
<xml_diff>
--- a/taskList.xlsx
+++ b/taskList.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vini2\Desktop\JJP Data Intelligence\Projetos\Projetos Ativos\3e Consulting\BI4U\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23796F1E-242F-4B5E-8517-0DEC5D2D9F5F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A964546-6110-4378-B30D-29BA0D6E635F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6C27AEC3-B6D4-43E8-A980-4A3197A4638C}"/>
   </bookViews>
@@ -125,12 +125,35 @@
         </r>
       </text>
     </comment>
+    <comment ref="F40" authorId="0" shapeId="0" xr:uid="{94CDCF0D-E596-400C-AF58-21910C733530}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+          </rPr>
+          <t>Vinícius Lavrador:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+          </rPr>
+          <t xml:space="preserve">
+Estudar o formset de Dependentes.
+Estudar adicionar Dependentes 7 Dependentes como formulário padrão no Criar Funcionario WizardForm</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
   <si>
     <t>Tela inicial do sistema, deve ser aquela azul que lhe passei com o logo da GAP no meio.</t>
   </si>
@@ -264,9 +287,6 @@
     <t>Ajustar Formulários de Lançamentos Receita e Despesa para o Valor total refletir a soma dos produtos e serviços menos o percentual de desconto</t>
   </si>
   <si>
-    <t>Ao Abrir o Menu, Fechar os Submenus de Lançamentos</t>
-  </si>
-  <si>
     <t xml:space="preserve">No Fluxo de Caixa, mostrar visões dos seguintes períodos: -Diário(Escolhe Mês e Ano), Semana(Sumarização por Semana, Escolhe mês e ano), Ultimos 3 Meses(Sumarização por Mês, sem escolhas), Ultimos 6 Meses (idem ao anterior), Ultimos 12 Meses(Sumarização por Mês) </t>
   </si>
   <si>
@@ -279,14 +299,59 @@
     <t>Adicionar Dependentes no Módulo Funcionário</t>
   </si>
   <si>
-    <t>Pesquisar e Criar Método de exportação das diferentes vizualizações do módulo financeiro</t>
+    <t>Pesquisar e Criar Método de exportação das diferentes vizualizações do módulo financeiro - Exportar como CSV</t>
+  </si>
+  <si>
+    <t>Ligar na KingHost e Confirmar Informações do Servidor (Plano 2) - Tel: 4003-5464</t>
+  </si>
+  <si>
+    <t>Estudar Migração MySQL</t>
+  </si>
+  <si>
+    <t>Verificar com a KingHost o IP do Host e dos FailSafes</t>
+  </si>
+  <si>
+    <t>Criar Documentação do Projeto + Guia de Usuário</t>
+  </si>
+  <si>
+    <t>Ajustar data de Criação do Funcionario, Timestam em BasicInfo</t>
+  </si>
+  <si>
+    <t>Arrumar Desligamento, caso de CPF vazio</t>
+  </si>
+  <si>
+    <t>Ao Abrir o Menu, Fechar os Submenus de Lançamentos (Ajustar Show &amp; Hide)</t>
+  </si>
+  <si>
+    <t>Adicionar Identificador de Lancamento, Para que ao visualizar os lancamentos possamos identificar o lancamento de maneira clara. Ao clicar na linha, abrimos o lancamento detalhado.</t>
+  </si>
+  <si>
+    <t>Adicionar modal de Reativação de Funcionário</t>
+  </si>
+  <si>
+    <t>Alterar desligamento para status</t>
+  </si>
+  <si>
+    <t>Arrumar o visualizar lancamentos para trazer o identificador receita na tabela</t>
+  </si>
+  <si>
+    <t>Incluir Botão de Visualização de Detalhes no Visualizar Lancamentos que Traz um modal com os Detalhes do Lancamento</t>
+  </si>
+  <si>
+    <t>No detalhamento trazer botão de exclusão do lancamento</t>
+  </si>
+  <si>
+    <t>No visualizar lancamento incluir segregacao de periodo idem item 35</t>
+  </si>
+  <si>
+    <t>Terminar alteração de círculos para retângulos nos menus de aplicativo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,8 +402,19 @@
       <name val="Segoe UI"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -360,6 +436,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -418,7 +500,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -483,41 +565,86 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -834,10 +961,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44BB84BF-369C-45E9-A482-8E63367EB510}">
-  <dimension ref="A1:M40"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J47" sqref="J47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -865,11 +992,11 @@
       <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
+      <c r="I2" s="46"/>
+      <c r="J2" s="46"/>
     </row>
     <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -894,8 +1021,8 @@
         <v>18</v>
       </c>
       <c r="M3" s="5">
-        <f>SUM(H3:H28)/COUNTA(H3:H28)</f>
-        <v>0.92307692307692313</v>
+        <f>SUM(H3:H54)/COUNTA(H3:H54)</f>
+        <v>0.57692307692307687</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -913,7 +1040,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="12">
-        <f t="shared" ref="I4:I40" si="0">H4</f>
+        <f t="shared" ref="I4:I54" si="0">H4</f>
         <v>1</v>
       </c>
       <c r="J4" s="13"/>
@@ -1396,13 +1523,13 @@
       <c r="J28" s="13"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E29" s="26">
+      <c r="E29" s="25">
         <v>27</v>
       </c>
-      <c r="F29" s="25" t="s">
+      <c r="F29" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="24">
+      <c r="G29" s="23">
         <v>43574</v>
       </c>
       <c r="H29" s="8">
@@ -1415,16 +1542,16 @@
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E30" s="29">
+      <c r="E30" s="28">
         <v>28</v>
       </c>
-      <c r="F30" s="30" t="s">
+      <c r="F30" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="G30" s="31">
+      <c r="G30" s="30">
         <v>43574</v>
       </c>
-      <c r="H30" s="32">
+      <c r="H30" s="31">
         <v>-1</v>
       </c>
       <c r="I30" s="12">
@@ -1434,16 +1561,16 @@
       <c r="J30" s="20"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E31" s="29">
+      <c r="E31" s="28">
         <v>29</v>
       </c>
-      <c r="F31" s="30" t="s">
+      <c r="F31" s="29" t="s">
         <v>39</v>
       </c>
-      <c r="G31" s="31">
+      <c r="G31" s="30">
         <v>43574</v>
       </c>
-      <c r="H31" s="32">
+      <c r="H31" s="31">
         <v>-1</v>
       </c>
       <c r="I31" s="12">
@@ -1453,16 +1580,16 @@
       <c r="J31" s="20"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E32" s="29">
+      <c r="E32" s="28">
         <v>30</v>
       </c>
-      <c r="F32" s="30" t="s">
+      <c r="F32" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="G32" s="31">
+      <c r="G32" s="30">
         <v>43574</v>
       </c>
-      <c r="H32" s="32">
+      <c r="H32" s="31">
         <v>-1</v>
       </c>
       <c r="I32" s="12">
@@ -1471,69 +1598,79 @@
       </c>
       <c r="J32" s="20"/>
     </row>
-    <row r="33" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E33" s="27">
+    <row r="33" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D33" s="37">
+        <v>1</v>
+      </c>
+      <c r="E33" s="25">
         <v>31</v>
       </c>
-      <c r="F33" s="33" t="s">
+      <c r="F33" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="21">
+      <c r="G33" s="23">
         <v>43574</v>
       </c>
-      <c r="H33" s="3">
-        <v>0</v>
+      <c r="H33" s="41">
+        <v>1</v>
       </c>
       <c r="I33" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J33" s="20"/>
-    </row>
-    <row r="34" spans="5:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E34" s="28">
+        <v>1</v>
+      </c>
+      <c r="J33" s="21">
+        <v>43595</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E34" s="7">
         <v>32</v>
       </c>
-      <c r="F34" s="23" t="s">
+      <c r="F34" s="24" t="s">
         <v>43</v>
       </c>
-      <c r="G34" s="16">
+      <c r="G34" s="15">
         <v>43574</v>
       </c>
-      <c r="H34" s="3">
-        <v>0</v>
+      <c r="H34" s="8">
+        <v>1</v>
       </c>
       <c r="I34" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J34" s="20"/>
     </row>
-    <row r="35" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E35" s="27">
+    <row r="35" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D35" s="1">
+        <v>1</v>
+      </c>
+      <c r="E35" s="25">
         <v>33</v>
       </c>
-      <c r="F35" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="G35" s="21">
+      <c r="F35" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="G35" s="23">
         <v>43574</v>
       </c>
-      <c r="H35" s="3">
-        <v>0</v>
+      <c r="H35" s="8">
+        <v>1</v>
       </c>
       <c r="I35" s="12">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="20"/>
-    </row>
-    <row r="36" spans="5:10" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="E36" s="28">
+        <v>1</v>
+      </c>
+      <c r="J35" s="21">
+        <v>43595</v>
+      </c>
+    </row>
+    <row r="36" spans="4:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E36" s="27">
         <v>34</v>
       </c>
-      <c r="F36" s="23" t="s">
-        <v>49</v>
+      <c r="F36" s="22" t="s">
+        <v>48</v>
       </c>
       <c r="G36" s="16">
         <v>43574</v>
@@ -1547,50 +1684,50 @@
       </c>
       <c r="J36" s="20"/>
     </row>
-    <row r="37" spans="5:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="E37" s="28">
+    <row r="37" spans="4:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E37" s="42">
         <v>35</v>
       </c>
-      <c r="F37" s="23" t="s">
+      <c r="F37" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="G37" s="44">
+        <v>43574</v>
+      </c>
+      <c r="H37" s="11">
+        <v>0</v>
+      </c>
+      <c r="I37" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J37" s="20"/>
+    </row>
+    <row r="38" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E38" s="25">
+        <v>36</v>
+      </c>
+      <c r="F38" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G37" s="16">
+      <c r="G38" s="23">
         <v>43574</v>
       </c>
-      <c r="H37" s="3">
-        <v>0</v>
-      </c>
-      <c r="I37" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J37" s="20"/>
-    </row>
-    <row r="38" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E38" s="27">
-        <v>36</v>
-      </c>
-      <c r="F38" s="23" t="s">
+      <c r="H38" s="8">
+        <v>1</v>
+      </c>
+      <c r="I38" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J38" s="20"/>
+    </row>
+    <row r="39" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E39" s="26">
+        <v>37</v>
+      </c>
+      <c r="F39" s="22" t="s">
         <v>46</v>
-      </c>
-      <c r="G38" s="21">
-        <v>43574</v>
-      </c>
-      <c r="H38" s="3">
-        <v>0</v>
-      </c>
-      <c r="I38" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J38" s="20"/>
-    </row>
-    <row r="39" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E39" s="27">
-        <v>37</v>
-      </c>
-      <c r="F39" s="23" t="s">
-        <v>47</v>
       </c>
       <c r="G39" s="21">
         <v>43574</v>
@@ -1604,30 +1741,327 @@
       </c>
       <c r="J39" s="20"/>
     </row>
-    <row r="40" spans="5:10" x14ac:dyDescent="0.3">
-      <c r="E40" s="27">
+    <row r="40" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E40" s="32">
         <v>38</v>
       </c>
-      <c r="F40" s="23" t="s">
+      <c r="F40" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="G40" s="34">
+        <v>43574</v>
+      </c>
+      <c r="H40" s="33">
+        <v>0</v>
+      </c>
+      <c r="I40" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J40" s="39">
+        <v>43600</v>
+      </c>
+    </row>
+    <row r="41" spans="4:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E41" s="20">
+        <v>39</v>
+      </c>
+      <c r="F41" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="G41" s="21">
+        <v>43593</v>
+      </c>
+      <c r="H41" s="3">
+        <v>0</v>
+      </c>
+      <c r="I41" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="20"/>
+    </row>
+    <row r="42" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E42" s="20">
+        <v>40</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G42" s="21">
+        <v>43593</v>
+      </c>
+      <c r="H42" s="3">
+        <v>0</v>
+      </c>
+      <c r="I42" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J42" s="20"/>
+    </row>
+    <row r="43" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E43" s="20">
+        <v>41</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G43" s="21">
+        <v>43593</v>
+      </c>
+      <c r="H43" s="3">
+        <v>0</v>
+      </c>
+      <c r="I43" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="20"/>
+    </row>
+    <row r="44" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E44" s="20">
+        <v>42</v>
+      </c>
+      <c r="F44" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="G44" s="21">
+        <v>43593</v>
+      </c>
+      <c r="H44" s="3">
+        <v>0</v>
+      </c>
+      <c r="I44" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J44" s="20"/>
+    </row>
+    <row r="45" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D45" s="1">
+        <v>1</v>
+      </c>
+      <c r="E45" s="45">
+        <v>43</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="G45" s="23">
+        <v>43593</v>
+      </c>
+      <c r="H45" s="8">
+        <v>1</v>
+      </c>
+      <c r="I45" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J45" s="21">
+        <v>43595</v>
+      </c>
+    </row>
+    <row r="46" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D46" s="1">
+        <v>1</v>
+      </c>
+      <c r="E46" s="45">
+        <v>44</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G46" s="23">
+        <v>43593</v>
+      </c>
+      <c r="H46" s="8">
+        <v>1</v>
+      </c>
+      <c r="I46" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J46" s="21">
+        <v>43595</v>
+      </c>
+    </row>
+    <row r="47" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="45">
+        <v>45</v>
+      </c>
+      <c r="F47" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G47" s="23">
+        <v>43593</v>
+      </c>
+      <c r="H47" s="8">
+        <v>1</v>
+      </c>
+      <c r="I47" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J47" s="21">
+        <v>43595</v>
+      </c>
+    </row>
+    <row r="48" spans="4:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="7">
+        <v>46</v>
+      </c>
+      <c r="F48" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="G48" s="47">
+        <v>43593</v>
+      </c>
+      <c r="H48" s="8">
+        <v>1</v>
+      </c>
+      <c r="I48" s="12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J48" s="21">
+        <v>43595</v>
+      </c>
+    </row>
+    <row r="49" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E49" s="35">
+        <v>47</v>
+      </c>
+      <c r="F49" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="G49" s="34">
+        <v>43593</v>
+      </c>
+      <c r="H49" s="33">
+        <v>0</v>
+      </c>
+      <c r="I49" s="48">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J49" s="21">
+        <v>43600</v>
+      </c>
+    </row>
+    <row r="50" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E50" s="20">
         <v>48</v>
       </c>
-      <c r="G40" s="21">
-        <v>43574</v>
-      </c>
-      <c r="H40" s="23">
-        <v>0</v>
-      </c>
-      <c r="I40" s="3">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J40" s="20"/>
+      <c r="F50" s="22" t="s">
+        <v>57</v>
+      </c>
+      <c r="G50" s="21">
+        <v>43593</v>
+      </c>
+      <c r="H50" s="22">
+        <v>0</v>
+      </c>
+      <c r="I50" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J50" s="21">
+        <v>43600</v>
+      </c>
+    </row>
+    <row r="51" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="45">
+        <v>49</v>
+      </c>
+      <c r="F51" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="G51" s="23">
+        <v>43593</v>
+      </c>
+      <c r="H51" s="24">
+        <v>0</v>
+      </c>
+      <c r="I51" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J51" s="21">
+        <v>43595</v>
+      </c>
+    </row>
+    <row r="52" spans="4:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E52" s="27">
+        <v>50</v>
+      </c>
+      <c r="F52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G52" s="38">
+        <v>43593</v>
+      </c>
+      <c r="H52" s="3">
+        <v>0</v>
+      </c>
+      <c r="I52" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J52" s="3"/>
+    </row>
+    <row r="53" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E53" s="20">
+        <v>60</v>
+      </c>
+      <c r="F53" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="G53" s="21">
+        <v>43593</v>
+      </c>
+      <c r="H53" s="22">
+        <v>0</v>
+      </c>
+      <c r="I53" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J53" s="20"/>
+    </row>
+    <row r="54" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E54" s="20">
+        <v>61</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>62</v>
+      </c>
+      <c r="G54" s="21">
+        <v>43593</v>
+      </c>
+      <c r="H54" s="22">
+        <v>0</v>
+      </c>
+      <c r="I54" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H2:J2"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:I40">
+  <conditionalFormatting sqref="I3:I54">
     <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>

</xml_diff>

<commit_message>
Changes on front-end and responsiveness
</commit_message>
<xml_diff>
--- a/taskList.xlsx
+++ b/taskList.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vini2\Desktop\JJP Data Intelligence\Projetos\Projetos Ativos\3e Consulting\BI4U\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A964546-6110-4378-B30D-29BA0D6E635F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D27BCC2-ADC1-422C-8DA9-72B858127CD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{6C27AEC3-B6D4-43E8-A980-4A3197A4638C}"/>
   </bookViews>
   <sheets>
     <sheet name="ToDo" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha1" sheetId="2" r:id="rId2"/>
+    <sheet name="Planilha1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="74">
   <si>
     <t>Tela inicial do sistema, deve ser aquela azul que lhe passei com o logo da GAP no meio.</t>
   </si>
@@ -251,21 +251,6 @@
     <t>Aguardando informações sobre metadados do backend virem do Thiago.</t>
   </si>
   <si>
-    <t>Boleto</t>
-  </si>
-  <si>
-    <t>Transferencia</t>
-  </si>
-  <si>
-    <t>Cartão de Débito</t>
-  </si>
-  <si>
-    <t>Cartão de Crédito</t>
-  </si>
-  <si>
-    <t>Dinheiro</t>
-  </si>
-  <si>
     <t>Alteração de Tipos de Forma de Pagamento</t>
   </si>
   <si>
@@ -278,9 +263,6 @@
     <t>Criação de 2 Grupos de Autorização e flag Staff no Django</t>
   </si>
   <si>
-    <t>No formulario de Receita e Despesa, teremos 2 paginas. A primeira com informações de Destalhes Financeiros (ID. Venda, Classificação De Receita, Produto ou Serviço, Quantidade, Valor Unitário do Produto ou Serviço)</t>
-  </si>
-  <si>
     <t>Ajustar Formulários de Lançamentos Receita e Despesa</t>
   </si>
   <si>
@@ -345,13 +327,157 @@
   </si>
   <si>
     <t>Terminar alteração de círculos para retângulos nos menus de aplicativo</t>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quando seleciono a opção  Estrangeiro na 1ª tela do cadastro ao chegar na 4ª tela mostra tela de erro</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quando seleciono a opção  Possui alguma deficiência na 1ª tela do cadastro ao chegar na 4ª tela mostra tela de erro</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quando seleciono a opção  É estagiário na 1ª tela do cadastro ao chegar na 6ª tela mostra tela de erro</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="7"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">         </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quando seleciono a opção  Possui outro emprego na 1ª tela do cadastro ao chegar na 6ª tela mostra tela de erro</t>
+    </r>
+  </si>
+  <si>
+    <t>ABA informações de contato, ao incluir no campo e-mail: “231313@com” ele não emiti msg de erro e nem passa para a outra tela</t>
+  </si>
+  <si>
+    <t>ABA Informações Bancária, permiti colocar letras no campo número da conta, corrigir</t>
+  </si>
+  <si>
+    <t>Incluir um botão de voltar para Home Page em todas as telas</t>
+  </si>
+  <si>
+    <t>Incluir um botão de salva e voltar para home page , pois,  hoje se eu entrar no cadastro do cliente e mudar 1 informação na 1ª tela preciso correr todas as telas até o final, é muito ruim isto.</t>
+  </si>
+  <si>
+    <t>Os 3 botões do sub-menu estão cortados na minha tela, parece que entraram mais do que deviam para a esquerda precisa rever.</t>
+  </si>
+  <si>
+    <t>No menu Financeiro, Ao fazer um lançamento e clicar no botão receita fixa, periodicidade mensal, apresenta uma tela de erro</t>
+  </si>
+  <si>
+    <t>No menu Financeiro, Ao fazer uma despesa e clicar no botão  fixa, periodicidade mensal, apresenta uma tela de erro</t>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ncluir um botão de Home Page em todas as telas do financeiro.</t>
+    </r>
+  </si>
+  <si>
+    <t>Incluir um botão de Home Page em todas as telas do financeiro.</t>
+  </si>
+  <si>
+    <t>Incluir um botão de voltar ou anterior dentro do modulo financeiro</t>
+  </si>
+  <si>
+    <t>Quando seleciono a opção na 1ª tela do cadastro ao chegar na 4ª tela mostra tela de erro</t>
+  </si>
+  <si>
+    <t>É complicado, verificar prioridade</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -413,8 +539,28 @@
       <color indexed="81"/>
       <name val="Segoe UI"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Symbol"/>
+      <family val="1"/>
+      <charset val="2"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -435,18 +581,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -495,12 +635,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -593,18 +748,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -643,8 +786,70 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -961,10 +1166,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44BB84BF-369C-45E9-A482-8E63367EB510}">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M64"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="J47" sqref="J47"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F59" sqref="F59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -986,17 +1191,17 @@
       <c r="E2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="42" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="46" t="s">
+      <c r="H2" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="46"/>
-      <c r="J2" s="46"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
     </row>
     <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
@@ -1021,8 +1226,8 @@
         <v>18</v>
       </c>
       <c r="M3" s="5">
-        <f>SUM(H3:H54)/COUNTA(H3:H54)</f>
-        <v>0.57692307692307687</v>
+        <f>SUM(H:H)/COUNTA(H:H)</f>
+        <v>0.58730158730158732</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
@@ -1040,7 +1245,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="12">
-        <f t="shared" ref="I4:I54" si="0">H4</f>
+        <f t="shared" ref="I4:I64" si="0">H4</f>
         <v>1</v>
       </c>
       <c r="J4" s="13"/>
@@ -1527,7 +1732,7 @@
         <v>27</v>
       </c>
       <c r="F29" s="24" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="G29" s="23">
         <v>43574</v>
@@ -1542,76 +1747,85 @@
       <c r="J29" s="20"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E30" s="28">
+      <c r="D30" s="1">
+        <v>-1</v>
+      </c>
+      <c r="E30" s="47">
         <v>28</v>
       </c>
-      <c r="F30" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="G30" s="30">
+      <c r="F30" s="39" t="s">
+        <v>33</v>
+      </c>
+      <c r="G30" s="35">
         <v>43574</v>
       </c>
-      <c r="H30" s="31">
+      <c r="H30" s="11">
+        <v>0</v>
+      </c>
+      <c r="I30" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="20"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D31" s="1">
         <v>-1</v>
       </c>
-      <c r="I30" s="12">
-        <f t="shared" si="0"/>
+      <c r="E31" s="47">
+        <v>29</v>
+      </c>
+      <c r="F31" s="39" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="35">
+        <v>43574</v>
+      </c>
+      <c r="H31" s="11">
+        <v>0</v>
+      </c>
+      <c r="I31" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J31" s="20"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="D32" s="1">
         <v>-1</v>
       </c>
-      <c r="J30" s="20"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E31" s="28">
-        <v>29</v>
-      </c>
-      <c r="F31" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="G31" s="30">
+      <c r="E32" s="47">
+        <v>30</v>
+      </c>
+      <c r="F32" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="G32" s="35">
         <v>43574</v>
       </c>
-      <c r="H31" s="31">
-        <v>-1</v>
-      </c>
-      <c r="I31" s="12">
-        <f t="shared" si="0"/>
-        <v>-1</v>
-      </c>
-      <c r="J31" s="20"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="E32" s="28">
-        <v>30</v>
-      </c>
-      <c r="F32" s="29" t="s">
-        <v>40</v>
-      </c>
-      <c r="G32" s="30">
-        <v>43574</v>
-      </c>
-      <c r="H32" s="31">
-        <v>-1</v>
+      <c r="H32" s="11">
+        <v>0</v>
       </c>
       <c r="I32" s="12">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="J32" s="20"/>
     </row>
     <row r="33" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="D33" s="37">
+      <c r="D33" s="33">
         <v>1</v>
       </c>
       <c r="E33" s="25">
         <v>31</v>
       </c>
-      <c r="F33" s="40" t="s">
-        <v>42</v>
+      <c r="F33" s="36" t="s">
+        <v>36</v>
       </c>
       <c r="G33" s="23">
         <v>43574</v>
       </c>
-      <c r="H33" s="41">
+      <c r="H33" s="37">
         <v>1</v>
       </c>
       <c r="I33" s="12">
@@ -1627,7 +1841,7 @@
         <v>32</v>
       </c>
       <c r="F34" s="24" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="G34" s="15">
         <v>43574</v>
@@ -1649,7 +1863,7 @@
         <v>33</v>
       </c>
       <c r="F35" s="24" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="G35" s="23">
         <v>43574</v>
@@ -1670,7 +1884,7 @@
         <v>34</v>
       </c>
       <c r="F36" s="22" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G36" s="16">
         <v>43574</v>
@@ -1685,13 +1899,13 @@
       <c r="J36" s="20"/>
     </row>
     <row r="37" spans="4:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="E37" s="42">
+      <c r="E37" s="38">
         <v>35</v>
       </c>
-      <c r="F37" s="43" t="s">
-        <v>44</v>
-      </c>
-      <c r="G37" s="44">
+      <c r="F37" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="G37" s="40">
         <v>43574</v>
       </c>
       <c r="H37" s="11">
@@ -1708,7 +1922,7 @@
         <v>36</v>
       </c>
       <c r="F38" s="24" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G38" s="23">
         <v>43574</v>
@@ -1727,7 +1941,7 @@
         <v>37</v>
       </c>
       <c r="F39" s="22" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="G39" s="21">
         <v>43574</v>
@@ -1742,23 +1956,23 @@
       <c r="J39" s="20"/>
     </row>
     <row r="40" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="E40" s="32">
+      <c r="E40" s="28">
         <v>38</v>
       </c>
-      <c r="F40" s="33" t="s">
-        <v>47</v>
-      </c>
-      <c r="G40" s="34">
+      <c r="F40" s="29" t="s">
+        <v>41</v>
+      </c>
+      <c r="G40" s="30">
         <v>43574</v>
       </c>
-      <c r="H40" s="33">
+      <c r="H40" s="29">
         <v>0</v>
       </c>
       <c r="I40" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="J40" s="39">
+      <c r="J40" s="35">
         <v>43600</v>
       </c>
     </row>
@@ -1766,8 +1980,8 @@
       <c r="E41" s="20">
         <v>39</v>
       </c>
-      <c r="F41" s="36" t="s">
-        <v>49</v>
+      <c r="F41" s="32" t="s">
+        <v>43</v>
       </c>
       <c r="G41" s="21">
         <v>43593</v>
@@ -1786,7 +2000,7 @@
         <v>40</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="G42" s="21">
         <v>43593</v>
@@ -1805,7 +2019,7 @@
         <v>41</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="G43" s="21">
         <v>43593</v>
@@ -1824,7 +2038,7 @@
         <v>42</v>
       </c>
       <c r="F44" s="22" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G44" s="21">
         <v>43593</v>
@@ -1842,11 +2056,11 @@
       <c r="D45" s="1">
         <v>1</v>
       </c>
-      <c r="E45" s="45">
+      <c r="E45" s="41">
         <v>43</v>
       </c>
       <c r="F45" s="8" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="G45" s="23">
         <v>43593</v>
@@ -1866,11 +2080,11 @@
       <c r="D46" s="1">
         <v>1</v>
       </c>
-      <c r="E46" s="45">
+      <c r="E46" s="41">
         <v>44</v>
       </c>
       <c r="F46" s="8" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="G46" s="23">
         <v>43593</v>
@@ -1890,11 +2104,11 @@
       <c r="D47" s="1">
         <v>1</v>
       </c>
-      <c r="E47" s="45">
+      <c r="E47" s="41">
         <v>45</v>
       </c>
       <c r="F47" s="8" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="G47" s="23">
         <v>43593</v>
@@ -1918,9 +2132,9 @@
         <v>46</v>
       </c>
       <c r="F48" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G48" s="47">
+        <v>50</v>
+      </c>
+      <c r="G48" s="43">
         <v>43593</v>
       </c>
       <c r="H48" s="8">
@@ -1935,19 +2149,19 @@
       </c>
     </row>
     <row r="49" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="E49" s="35">
+      <c r="E49" s="31">
         <v>47</v>
       </c>
-      <c r="F49" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="G49" s="34">
+      <c r="F49" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="G49" s="30">
         <v>43593</v>
       </c>
-      <c r="H49" s="33">
-        <v>0</v>
-      </c>
-      <c r="I49" s="48">
+      <c r="H49" s="29">
+        <v>0</v>
+      </c>
+      <c r="I49" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1960,7 +2174,7 @@
         <v>48</v>
       </c>
       <c r="F50" s="22" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="G50" s="21">
         <v>43593</v>
@@ -1980,11 +2194,11 @@
       <c r="D51" s="1">
         <v>1</v>
       </c>
-      <c r="E51" s="45">
+      <c r="E51" s="41">
         <v>49</v>
       </c>
       <c r="F51" s="24" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G51" s="23">
         <v>43593</v>
@@ -2005,9 +2219,9 @@
         <v>50</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G52" s="38">
+        <v>54</v>
+      </c>
+      <c r="G52" s="34">
         <v>43593</v>
       </c>
       <c r="H52" s="3">
@@ -2021,10 +2235,10 @@
     </row>
     <row r="53" spans="4:10" x14ac:dyDescent="0.3">
       <c r="E53" s="20">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F53" s="22" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="G53" s="21">
         <v>43593</v>
@@ -2038,30 +2252,222 @@
       </c>
       <c r="J53" s="20"/>
     </row>
-    <row r="54" spans="4:10" x14ac:dyDescent="0.3">
-      <c r="E54" s="20">
+    <row r="54" spans="4:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E54" s="49">
+        <v>52</v>
+      </c>
+      <c r="F54" s="50" t="s">
+        <v>56</v>
+      </c>
+      <c r="G54" s="51">
+        <v>43593</v>
+      </c>
+      <c r="H54" s="50">
+        <v>0</v>
+      </c>
+      <c r="I54" s="52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J54" s="49"/>
+    </row>
+    <row r="55" spans="4:10" ht="29.4" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="E55" s="53">
+        <v>53</v>
+      </c>
+      <c r="F55" s="54" t="s">
+        <v>62</v>
+      </c>
+      <c r="G55" s="55">
+        <v>43601</v>
+      </c>
+      <c r="H55" s="56">
+        <v>1</v>
+      </c>
+      <c r="I55" s="56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J55" s="48"/>
+    </row>
+    <row r="56" spans="4:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E56" s="61">
+        <v>54</v>
+      </c>
+      <c r="F56" s="61" t="s">
+        <v>63</v>
+      </c>
+      <c r="G56" s="62">
+        <v>43601</v>
+      </c>
+      <c r="H56" s="63">
+        <v>0</v>
+      </c>
+      <c r="I56" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J56" s="20"/>
+    </row>
+    <row r="57" spans="4:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E57" s="61">
+        <v>55</v>
+      </c>
+      <c r="F57" s="61" t="s">
+        <v>72</v>
+      </c>
+      <c r="G57" s="62">
+        <v>43601</v>
+      </c>
+      <c r="H57" s="63">
+        <v>0</v>
+      </c>
+      <c r="I57" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J57" s="20"/>
+    </row>
+    <row r="58" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E58" s="65">
+        <v>56</v>
+      </c>
+      <c r="F58" s="61" t="s">
+        <v>64</v>
+      </c>
+      <c r="G58" s="62">
+        <v>43601</v>
+      </c>
+      <c r="H58" s="63">
+        <v>0</v>
+      </c>
+      <c r="I58" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J58" s="20"/>
+    </row>
+    <row r="59" spans="4:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E59" s="61">
+        <v>57</v>
+      </c>
+      <c r="F59" s="61" t="s">
+        <v>65</v>
+      </c>
+      <c r="G59" s="62">
+        <v>43601</v>
+      </c>
+      <c r="H59" s="63">
+        <v>0</v>
+      </c>
+      <c r="I59" s="64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J59" s="20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="60" spans="4:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E60" s="41">
+        <v>58</v>
+      </c>
+      <c r="F60" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="G60" s="23">
+        <v>43601</v>
+      </c>
+      <c r="H60" s="8">
+        <v>1</v>
+      </c>
+      <c r="I60" s="56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J60" s="20"/>
+    </row>
+    <row r="61" spans="4:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E61" s="7">
+        <v>59</v>
+      </c>
+      <c r="F61" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="G61" s="23">
+        <v>43601</v>
+      </c>
+      <c r="H61" s="8">
+        <v>1</v>
+      </c>
+      <c r="I61" s="56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J61" s="20"/>
+    </row>
+    <row r="62" spans="4:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E62" s="41">
+        <v>60</v>
+      </c>
+      <c r="F62" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="G62" s="23">
+        <v>43601</v>
+      </c>
+      <c r="H62" s="8">
+        <v>1</v>
+      </c>
+      <c r="I62" s="56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="J62" s="20"/>
+    </row>
+    <row r="63" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E63" s="57">
         <v>61</v>
       </c>
-      <c r="F54" s="22" t="s">
+      <c r="F63" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="G63" s="58">
+        <v>43601</v>
+      </c>
+      <c r="H63" s="59">
+        <v>0</v>
+      </c>
+      <c r="I63" s="60">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J63" s="20"/>
+    </row>
+    <row r="64" spans="4:10" x14ac:dyDescent="0.3">
+      <c r="E64" s="66">
         <v>62</v>
       </c>
-      <c r="G54" s="21">
-        <v>43593</v>
-      </c>
-      <c r="H54" s="22">
-        <v>0</v>
-      </c>
-      <c r="I54" s="12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J54" s="20"/>
+      <c r="F64" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="G64" s="58">
+        <v>43601</v>
+      </c>
+      <c r="H64" s="59">
+        <v>0</v>
+      </c>
+      <c r="I64" s="12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J64" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H2:J2"/>
   </mergeCells>
-  <conditionalFormatting sqref="I3:I54">
+  <conditionalFormatting sqref="I3:I64">
     <cfRule type="iconSet" priority="3">
       <iconSet iconSet="3Symbols" showValue="0">
         <cfvo type="percent" val="0"/>
@@ -2077,47 +2483,72 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{134A7412-1C13-47AD-96AC-2FA85A2170B3}">
-  <dimension ref="A1:F5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1376F55E-4928-4FAD-83AB-B42E3EAC078A}">
+  <dimension ref="A2:A22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A5"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="40.6640625" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>36</v>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="45" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="45" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="45" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="45" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="46" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="46" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="46" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="46" t="s">
+        <v>71</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>